<commit_message>
Updated language results in lab3 xlsx
</commit_message>
<xml_diff>
--- a/results/lab3.xlsx
+++ b/results/lab3.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="35">
   <si>
     <t>norm_wiki_en,txt</t>
   </si>
@@ -85,7 +85,7 @@
     <t>sample0,txt</t>
   </si>
   <si>
-    <t>~OK?</t>
+    <t>OK - volapük</t>
   </si>
   <si>
     <t>odchylenie</t>
@@ -94,13 +94,19 @@
     <t>sample1,txt</t>
   </si>
   <si>
-    <t>OK</t>
+    <t>OK - jawajski</t>
   </si>
   <si>
     <t>sample2,txt</t>
   </si>
   <si>
+    <t>OK - aragoński</t>
+  </si>
+  <si>
     <t>sample3,txt</t>
+  </si>
+  <si>
+    <t>OK - ilokano</t>
   </si>
   <si>
     <t>sample4,txt</t>
@@ -2011,7 +2017,7 @@
         <v>28</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="227">
@@ -2221,7 +2227,7 @@
     </row>
     <row r="251">
       <c r="A251" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="252">
@@ -2234,7 +2240,7 @@
         <v>8</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="254">
@@ -2434,10 +2440,10 @@
     </row>
     <row r="276">
       <c r="A276" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="277">
@@ -2647,7 +2653,7 @@
     </row>
     <row r="301">
       <c r="A301" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="302">
@@ -2660,7 +2666,7 @@
         <v>8</v>
       </c>
       <c r="E303" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="304">

</xml_diff>